<commit_message>
Moved graphs to excell
</commit_message>
<xml_diff>
--- a/Task_5/systems/systems.xlsx
+++ b/Task_5/systems/systems.xlsx
@@ -1,21 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28615"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/AlexTheLion/Desktop/PythonCourse_SystemProgramming/Task_5/systems/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="5">
   <si>
     <t>Линейная</t>
   </si>
@@ -35,20 +47,19 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -64,19 +75,618 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="113"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="13"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Linear</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet!$B$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet!$A$3:$A$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>80.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet!$B$4:$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>80.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>160.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-1813496544"/>
+        <c:axId val="-1813494496"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-1813496544"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-1813494496"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-1813494496"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-1813496544"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="113"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="13"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Dynamic</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet!$D$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0,455978889</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+            <a:effectLst>
+              <a:softEdge rad="749300"/>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet!$C$3:$C$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>80.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>160.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet!$D$4:$D$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1.912945250727628</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.745113160479349</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.00611134607662478</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.219425258379005</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-1813268064"/>
+        <c:axId val="-1813131232"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-1813268064"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-1813131232"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-1813131232"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-1813268064"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="113"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="13"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Anything</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet!$F$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0,455978889</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+            <a:effectLst>
+              <a:softEdge rad="457200"/>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet!$E$3:$E$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>80.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet!$F$4:$F$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1.912945250727628</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.745113160479349</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.00611134607662478</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.219425258379005</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-1812090640"/>
+        <c:axId val="-1812089008"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-1812090640"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-1812089008"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-1812089008"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-1812090640"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="5400000" cy="2700000"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="5400000" cy="2700000"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="5400000" cy="2700000"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -363,31 +973,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Y2" sqref="Y2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="3"/>
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="D1" s="3"/>
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="F1" s="3"/>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -407,104 +1016,104 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
-      <c r="A3" t="n">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3">
         <v>5</v>
       </c>
-      <c r="B3" t="n">
+      <c r="B3">
         <v>10</v>
       </c>
-      <c r="C3" t="n">
+      <c r="C3">
         <v>10</v>
       </c>
-      <c r="D3" t="n">
-        <v>0.4559788891106301</v>
-      </c>
-      <c r="E3" t="n">
+      <c r="D3">
+        <v>0.45597888911063011</v>
+      </c>
+      <c r="E3">
         <v>5</v>
       </c>
-      <c r="F3" t="n">
-        <v>0.4559788891106301</v>
+      <c r="F3">
+        <v>0.45597888911063011</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
-      <c r="A4" t="n">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4">
         <v>10</v>
       </c>
-      <c r="B4" t="n">
+      <c r="B4">
         <v>20</v>
       </c>
-      <c r="C4" t="n">
+      <c r="C4">
         <v>20</v>
       </c>
-      <c r="D4" t="n">
-        <v>1.912945250727628</v>
-      </c>
-      <c r="E4" t="n">
+      <c r="D4">
+        <v>1.9129452507276281</v>
+      </c>
+      <c r="E4">
         <v>10</v>
       </c>
-      <c r="F4" t="n">
-        <v>1.912945250727628</v>
+      <c r="F4">
+        <v>1.9129452507276281</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
-      <c r="A5" t="n">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5">
         <v>20</v>
       </c>
-      <c r="B5" t="n">
+      <c r="B5">
         <v>40</v>
       </c>
-      <c r="C5" t="n">
+      <c r="C5">
         <v>40</v>
       </c>
-      <c r="D5" t="n">
-        <v>1.745113160479349</v>
-      </c>
-      <c r="E5" t="n">
+      <c r="D5">
+        <v>1.7451131604793491</v>
+      </c>
+      <c r="E5">
         <v>20</v>
       </c>
-      <c r="F5" t="n">
-        <v>1.745113160479349</v>
+      <c r="F5">
+        <v>1.7451131604793491</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
-      <c r="A6" t="n">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6">
         <v>40</v>
       </c>
-      <c r="B6" t="n">
+      <c r="B6">
         <v>80</v>
       </c>
-      <c r="C6" t="n">
+      <c r="C6">
         <v>80</v>
       </c>
-      <c r="D6" t="n">
-        <v>0.00611134607662478</v>
-      </c>
-      <c r="E6" t="n">
+      <c r="D6">
+        <v>6.1113460766247796E-3</v>
+      </c>
+      <c r="E6">
         <v>40</v>
       </c>
-      <c r="F6" t="n">
-        <v>0.00611134607662478</v>
+      <c r="F6">
+        <v>6.1113460766247796E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
-      <c r="A7" t="n">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7">
         <v>80</v>
       </c>
-      <c r="B7" t="n">
+      <c r="B7">
         <v>160</v>
       </c>
-      <c r="C7" t="n">
+      <c r="C7">
         <v>160</v>
       </c>
-      <c r="D7" t="n">
-        <v>1.219425258379005</v>
-      </c>
-      <c r="E7" t="n">
+      <c r="D7">
+        <v>1.2194252583790051</v>
+      </c>
+      <c r="E7">
         <v>80</v>
       </c>
-      <c r="F7" t="n">
-        <v>1.219425258379005</v>
+      <c r="F7">
+        <v>1.2194252583790051</v>
       </c>
     </row>
   </sheetData>
@@ -513,6 +1122,7 @@
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:F1"/>
   </mergeCells>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>